<commit_message>
regenerate project files to try and fix test failure
</commit_message>
<xml_diff>
--- a/project/excel/ingest_metadata.xlsx
+++ b/project/excel/ingest_metadata.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="IngestMetadata" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="IngestMetadataFile" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -424,17 +424,17 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>title</t>
+          <t>file_name</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>created_by</t>
+          <t>file_created_by</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>creation_date</t>
+          <t>file_creation_date</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
@@ -444,97 +444,97 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>ingest_guide_url</t>
+          <t>source_infores_id</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>source_infores_id</t>
+          <t>source_data_version</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>source_license</t>
+          <t>source_access_date</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>source_data_version</t>
+          <t>source_access_urls</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>source_publication_date</t>
+          <t>source_file_names</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>source_download_date</t>
+          <t>target_name</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>source_access_urls</t>
+          <t>target_creation_date</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>source_data_formats</t>
+          <t>target_format</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>source_data_files</t>
+          <t>target_model</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>target_title</t>
+          <t>target_model_url</t>
         </is>
       </c>
       <c r="O1" t="inlineStr">
         <is>
-          <t>target_type</t>
+          <t>target_data_model_version</t>
         </is>
       </c>
       <c r="P1" t="inlineStr">
         <is>
-          <t>target_data_version</t>
+          <t>node_normalizer</t>
         </is>
       </c>
       <c r="Q1" t="inlineStr">
         <is>
-          <t>target_creation_date</t>
+          <t>node_normalizer_version</t>
         </is>
       </c>
       <c r="R1" t="inlineStr">
         <is>
-          <t>target_license</t>
+          <t>node_normalizer_url</t>
         </is>
       </c>
       <c r="S1" t="inlineStr">
         <is>
-          <t>target_data_format</t>
+          <t>total_edge_count</t>
         </is>
       </c>
       <c r="T1" t="inlineStr">
         <is>
-          <t>target_data_model</t>
+          <t>total_node_count</t>
         </is>
       </c>
       <c r="U1" t="inlineStr">
         <is>
-          <t>target_data_model_version</t>
+          <t>orphan_node_count</t>
         </is>
       </c>
       <c r="V1" t="inlineStr">
         <is>
-          <t>node_normalizer</t>
+          <t>node_categories</t>
         </is>
       </c>
       <c r="W1" t="inlineStr">
         <is>
-          <t>node_normalizer_version</t>
+          <t>edge_predicates</t>
         </is>
       </c>
     </row>

</xml_diff>